<commit_message>
孙际儒 20210611    Static hostname: yuyake-virtual-machine          Icon name: computer-vm            Chassis: vm         Machine ID: b971ed0d9c004e3d8fec2455825bf7a0            Boot ID: 2cc5dd8cac6f4ecda68957724fc6d2ad     Virtualization: vmware   Operating System: Ubuntu 20.04.3 LTS             Kernel: Linux 5.11.0-38-generic       Architecture: x86-64  10:41:25 up 13 min,  1 user,  load average: 2.49, 1.79, 1.33
</commit_message>
<xml_diff>
--- a/submit/Verilator中Warning无法清理说明.xlsx
+++ b/submit/Verilator中Warning无法清理说明.xlsx
@@ -496,7 +496,7 @@
   </sheetPr>
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B35" activeCellId="0" sqref="B35"/>
     </sheetView>
   </sheetViews>
@@ -921,7 +921,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.9921875" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.984375" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -944,7 +944,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.9921875" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.984375" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
孙际儒 20210611    Static hostname: yuyake-virtual-machine          Icon name: computer-vm            Chassis: vm         Machine ID: b971ed0d9c004e3d8fec2455825bf7a0            Boot ID: 3206134c56e34a32911ac9cd11139818     Virtualization: vmware   Operating System: Ubuntu 20.04.3 LTS             Kernel: Linux 5.11.0-38-generic       Architecture: x86-64  18:55:54 up  2:31,  1 user,  load average: 0.93, 0.64, 0.66
</commit_message>
<xml_diff>
--- a/submit/Verilator中Warning无法清理说明.xlsx
+++ b/submit/Verilator中Warning无法清理说明.xlsx
@@ -174,31 +174,31 @@
     <t xml:space="preserve">ysyx_210611.v:3589:44: Signal is not used: 'mem_rw_resp'</t>
   </si>
   <si>
-    <t xml:space="preserve">ysyx_210611.v:2796:35: Bits of signal are not used: 'itrp_info'[11:8,6:0]</t>
+    <t xml:space="preserve">ysyx_210611.v:2782:35: Bits of signal are not used: 'itrp_info'[11:8,6:0]</t>
   </si>
   <si>
     <t xml:space="preserve">仅实现了定时器中断，其他位预留给其他中断</t>
   </si>
   <si>
-    <t xml:space="preserve">ysyx_210611.v:2828:63: Bits of signal are not used: 'mie_rd_data'[63:12,10:8,6:4,2:0]</t>
+    <t xml:space="preserve">ysyx_210611.v:2814:63: Bits of signal are not used: 'mie_rd_data'[63:12,10:8,6:4,2:0]</t>
   </si>
   <si>
     <t xml:space="preserve">mie里与机器模式无关的信号未用</t>
   </si>
   <si>
-    <t xml:space="preserve">ysyx_210611.v:2828:76: Bits of signal are not used: 'mip_rd_data'[63:12,10:8,6:4,2:0]</t>
+    <t xml:space="preserve">ysyx_210611.v:2814:76: Bits of signal are not used: 'mip_rd_data'[63:12,10:8,6:4,2:0]</t>
   </si>
   <si>
     <t xml:space="preserve">mip里与机器模式无关的信号未用</t>
   </si>
   <si>
-    <t xml:space="preserve">ysyx_210611.v:2961:16: Bits of signal are not used: 'mem_reg_wr_ctrl'[2]</t>
+    <t xml:space="preserve">ysyx_210611.v:2947:16: Bits of signal are not used: 'mem_reg_wr_ctrl'[2]</t>
   </si>
   <si>
     <t xml:space="preserve">该信号是mem传递给wb的通用寄存器写入控制信号，也复用作为mem传递给ex的前递控制信号，第2位在前递中未用</t>
   </si>
   <si>
-    <t xml:space="preserve">ysyx_210611.v:2961:33: Bits of signal are not used: 'wb_reg_wr_ctrl'[2]</t>
+    <t xml:space="preserve">ysyx_210611.v:2947:33: Bits of signal are not used: 'wb_reg_wr_ctrl'[2]</t>
   </si>
   <si>
     <t xml:space="preserve">该信号是wb的通用寄存器写入控制信号，也复用作为wb传递给ex的前递控制信号，第2位在前递中未用</t>
@@ -496,8 +496,8 @@
   </sheetPr>
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B35" activeCellId="0" sqref="B35"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.9921875" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>